<commit_message>
- Updated factura's template - Fixed some cell-mapping bugs of InvoiceGenerator
</commit_message>
<xml_diff>
--- a/public/uploads/invoice/template.xlsx
+++ b/public/uploads/invoice/template.xlsx
@@ -186,48 +186,45 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="13">
   <si>
-    <t xml:space="preserve">Дата выписки</t>
+    <t xml:space="preserve">[Data elibirarii]</t>
   </si>
   <si>
-    <t xml:space="preserve">Дата поставки</t>
+    <t xml:space="preserve">[Data livrarii]</t>
   </si>
   <si>
     <t xml:space="preserve">-</t>
   </si>
   <si>
-    <t xml:space="preserve">Перевозчик</t>
+    <t xml:space="preserve">[Transportator]</t>
   </si>
   <si>
-    <t xml:space="preserve">Продавец</t>
+    <t xml:space="preserve">[c.f. / nr. TVA]</t>
   </si>
   <si>
-    <t xml:space="preserve">Покупатель</t>
+    <t xml:space="preserve">[Furnizor]</t>
   </si>
   <si>
-    <t xml:space="preserve">ф.к. / код НДС</t>
+    <t xml:space="preserve">[Cumparator]</t>
   </si>
   <si>
-    <t xml:space="preserve">Прилагаемые документы</t>
+    <t xml:space="preserve">[Documente anexate]</t>
   </si>
   <si>
-    <t xml:space="preserve">Пункт погрузки</t>
+    <t xml:space="preserve">[Punct incarcare]</t>
   </si>
   <si>
-    <t xml:space="preserve">Пункт разгрузки</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Item 1 name</t>
+    <t xml:space="preserve">[Punct descarcare]</t>
   </si>
   <si>
     <t xml:space="preserve">- </t>
   </si>
   <si>
-    <t xml:space="preserve">Director Vasea Pupkin</t>
+    <t xml:space="preserve">[Permis eliberarea</t>
   </si>
   <si>
-    <t xml:space="preserve">Vasea Pupkin</t>
+    <t xml:space="preserve">[Predat bunurile</t>
   </si>
 </sst>
 </file>
@@ -239,7 +236,7 @@
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
     <numFmt numFmtId="166" formatCode="#,##0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -274,6 +271,11 @@
       <charset val="204"/>
     </font>
     <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
       <sz val="7"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -328,7 +330,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -369,7 +371,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -409,7 +415,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -982,7 +988,7 @@
   <dimension ref="B1:T43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1063,9 +1069,8 @@
       <c r="L4" s="7"/>
       <c r="M4" s="8"/>
       <c r="N4" s="8"/>
-      <c r="O4" s="7" t="str">
-        <f aca="false">O6</f>
-        <v>ф.к. / код НДС</v>
+      <c r="O4" s="7" t="s">
+        <v>4</v>
       </c>
       <c r="P4" s="7"/>
       <c r="Q4" s="7"/>
@@ -1075,7 +1080,7 @@
     </row>
     <row r="5" customFormat="false" ht="17.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C5" s="9" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D5" s="9"/>
       <c r="E5" s="9"/>
@@ -1087,19 +1092,18 @@
       <c r="K5" s="9"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
-      <c r="O5" s="7" t="str">
-        <f aca="false">O6</f>
-        <v>ф.к. / код НДС</v>
-      </c>
-      <c r="P5" s="7"/>
-      <c r="Q5" s="7"/>
-      <c r="R5" s="7"/>
-      <c r="S5" s="7"/>
-      <c r="T5" s="7"/>
+      <c r="O5" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="P5" s="10"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="18.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C6" s="9" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D6" s="9"/>
       <c r="E6" s="9"/>
@@ -1111,48 +1115,48 @@
       <c r="K6" s="9"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
-      <c r="O6" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="P6" s="7"/>
-      <c r="Q6" s="7"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="7"/>
-      <c r="T6" s="7"/>
+      <c r="O6" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="P6" s="10"/>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="9.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C7" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="12"/>
-      <c r="M7" s="13" t="s">
+      <c r="C7" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F7" s="13"/>
+      <c r="M7" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="13"/>
-      <c r="O7" s="13"/>
-      <c r="P7" s="13"/>
-      <c r="Q7" s="13"/>
-      <c r="R7" s="13"/>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
+      <c r="N7" s="14"/>
+      <c r="O7" s="14"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="14"/>
+      <c r="R7" s="14"/>
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
     </row>
     <row r="8" customFormat="false" ht="8.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C8" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="M8" s="13"/>
-      <c r="N8" s="13"/>
-      <c r="O8" s="13"/>
-      <c r="P8" s="13"/>
-      <c r="Q8" s="13"/>
-      <c r="R8" s="13"/>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
+      <c r="C8" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="F8" s="13"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="14"/>
+      <c r="S8" s="14"/>
+      <c r="T8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="16.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="C9" s="9" t="s">
@@ -1166,80 +1170,80 @@
       <c r="I9" s="9"/>
       <c r="J9" s="9"/>
       <c r="K9" s="9"/>
-      <c r="N9" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="14"/>
-      <c r="S9" s="14"/>
-      <c r="T9" s="14"/>
+      <c r="N9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="O9" s="15"/>
+      <c r="P9" s="15"/>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="15"/>
+      <c r="S9" s="15"/>
+      <c r="T9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="48.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
-      <c r="L10" s="15"/>
-      <c r="M10" s="15"/>
-      <c r="N10" s="15"/>
-      <c r="O10" s="15"/>
-      <c r="P10" s="15"/>
-      <c r="Q10" s="15"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="F10" s="16"/>
+      <c r="G10" s="16"/>
+      <c r="I10" s="16"/>
+      <c r="J10" s="16"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="P10" s="16"/>
+      <c r="Q10" s="16"/>
     </row>
     <row r="11" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B11" s="9" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
-      <c r="E11" s="16" t="str">
-        <f aca="false">IF(ISBLANK( $B11), "-", "buc.")</f>
-        <v>buc.</v>
-      </c>
-      <c r="F11" s="17" t="n">
-        <v>10</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="18" t="n">
-        <f aca="false">IF(ISBLANK( $B11), "-", ROUNDUP($I11/$F11,2))</f>
-        <v>5</v>
-      </c>
-      <c r="I11" s="19" t="n">
-        <f aca="false">IF(ISBLANK( $B11), "-", $N11-$L11)</f>
-        <v>50</v>
-      </c>
-      <c r="J11" s="19"/>
-      <c r="K11" s="20" t="str">
-        <f aca="false">IF(ISBLANK( $B11), "-", "20%")</f>
-        <v>20%</v>
-      </c>
-      <c r="L11" s="19" t="n">
-        <f aca="false">IF(ISBLANK( $B11), "-", ROUNDUP($N11/6,2))</f>
-        <v>10</v>
-      </c>
-      <c r="M11" s="19"/>
-      <c r="N11" s="19" t="n">
-        <v>60</v>
-      </c>
-      <c r="O11" s="19"/>
-      <c r="P11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="R11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S11" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T11" s="14" t="s">
+      <c r="E11" s="17" t="str">
+        <f aca="false">IF($B11="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="19" t="str">
+        <f aca="false">IF($B11="-", "-", ROUNDUP($I11/$F11,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I11" s="20" t="str">
+        <f aca="false">IF($B11="-", "-", $N11-$L11)</f>
+        <v>-</v>
+      </c>
+      <c r="J11" s="20"/>
+      <c r="K11" s="21" t="str">
+        <f aca="false">IF($B11="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L11" s="20" t="str">
+        <f aca="false">IF($B11="-", "-", ROUNDUP($N11/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M11" s="20"/>
+      <c r="N11" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O11" s="20"/>
+      <c r="P11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T11" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1249,42 +1253,47 @@
       </c>
       <c r="C12" s="9"/>
       <c r="D12" s="9"/>
-      <c r="E12" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G12" s="17"/>
-      <c r="H12" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J12" s="19"/>
-      <c r="K12" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M12" s="19"/>
-      <c r="N12" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O12" s="19"/>
-      <c r="P12" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S12" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T12" s="14" t="s">
+      <c r="E12" s="17" t="str">
+        <f aca="false">IF($B12="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="19" t="str">
+        <f aca="false">IF($B12="-", "-", ROUNDUP($I12/$F12,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I12" s="20" t="str">
+        <f aca="false">IF($B12="-", "-", $N12-$L12)</f>
+        <v>-</v>
+      </c>
+      <c r="J12" s="20"/>
+      <c r="K12" s="21" t="str">
+        <f aca="false">IF($B12="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L12" s="20" t="str">
+        <f aca="false">IF($B12="-", "-", ROUNDUP($N12/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O12" s="20"/>
+      <c r="P12" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q12" s="15"/>
+      <c r="R12" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S12" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T12" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1294,42 +1303,47 @@
       </c>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
-      <c r="E13" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G13" s="17"/>
-      <c r="H13" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J13" s="19"/>
-      <c r="K13" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M13" s="19"/>
-      <c r="N13" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O13" s="19"/>
-      <c r="P13" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q13" s="14"/>
-      <c r="R13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S13" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T13" s="14" t="s">
+      <c r="E13" s="17" t="str">
+        <f aca="false">IF($B13="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="19" t="str">
+        <f aca="false">IF($B13="-", "-", ROUNDUP($I13/$F13,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I13" s="20" t="str">
+        <f aca="false">IF($B13="-", "-", $N13-$L13)</f>
+        <v>-</v>
+      </c>
+      <c r="J13" s="20"/>
+      <c r="K13" s="21" t="str">
+        <f aca="false">IF($B13="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L13" s="20" t="str">
+        <f aca="false">IF($B13="-", "-", ROUNDUP($N13/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M13" s="20"/>
+      <c r="N13" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O13" s="20"/>
+      <c r="P13" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q13" s="15"/>
+      <c r="R13" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S13" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T13" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1339,42 +1353,47 @@
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="9"/>
-      <c r="E14" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J14" s="19"/>
-      <c r="K14" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M14" s="19"/>
-      <c r="N14" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O14" s="19"/>
-      <c r="P14" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S14" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T14" s="14" t="s">
+      <c r="E14" s="17" t="str">
+        <f aca="false">IF($B14="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="19" t="str">
+        <f aca="false">IF($B14="-", "-", ROUNDUP($I14/$F14,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I14" s="20" t="str">
+        <f aca="false">IF($B14="-", "-", $N14-$L14)</f>
+        <v>-</v>
+      </c>
+      <c r="J14" s="20"/>
+      <c r="K14" s="21" t="str">
+        <f aca="false">IF($B14="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L14" s="20" t="str">
+        <f aca="false">IF($B14="-", "-", ROUNDUP($N14/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M14" s="20"/>
+      <c r="N14" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O14" s="20"/>
+      <c r="P14" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T14" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1384,42 +1403,47 @@
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G15" s="17"/>
-      <c r="H15" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J15" s="19"/>
-      <c r="K15" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M15" s="19"/>
-      <c r="N15" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O15" s="19"/>
-      <c r="P15" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S15" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T15" s="14" t="s">
+      <c r="E15" s="17" t="str">
+        <f aca="false">IF($B15="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="19" t="str">
+        <f aca="false">IF($B15="-", "-", ROUNDUP($I15/$F15,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I15" s="20" t="str">
+        <f aca="false">IF($B15="-", "-", $N15-$L15)</f>
+        <v>-</v>
+      </c>
+      <c r="J15" s="20"/>
+      <c r="K15" s="21" t="str">
+        <f aca="false">IF($B15="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L15" s="20" t="str">
+        <f aca="false">IF($B15="-", "-", ROUNDUP($N15/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M15" s="20"/>
+      <c r="N15" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O15" s="20"/>
+      <c r="P15" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q15" s="15"/>
+      <c r="R15" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S15" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1429,42 +1453,47 @@
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="17"/>
-      <c r="H16" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="19"/>
-      <c r="K16" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16" s="19"/>
-      <c r="N16" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O16" s="19"/>
-      <c r="P16" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q16" s="14"/>
-      <c r="R16" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S16" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T16" s="14" t="s">
+      <c r="E16" s="17" t="str">
+        <f aca="false">IF($B16="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="19" t="str">
+        <f aca="false">IF($B16="-", "-", ROUNDUP($I16/$F16,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I16" s="20" t="str">
+        <f aca="false">IF($B16="-", "-", $N16-$L16)</f>
+        <v>-</v>
+      </c>
+      <c r="J16" s="20"/>
+      <c r="K16" s="21" t="str">
+        <f aca="false">IF($B16="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L16" s="20" t="str">
+        <f aca="false">IF($B16="-", "-", ROUNDUP($N16/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M16" s="20"/>
+      <c r="N16" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" s="20"/>
+      <c r="P16" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q16" s="15"/>
+      <c r="R16" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T16" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1474,42 +1503,47 @@
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
-      <c r="E17" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G17" s="17"/>
-      <c r="H17" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J17" s="19"/>
-      <c r="K17" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M17" s="19"/>
-      <c r="N17" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O17" s="19"/>
-      <c r="P17" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q17" s="14"/>
-      <c r="R17" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S17" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T17" s="14" t="s">
+      <c r="E17" s="17" t="str">
+        <f aca="false">IF($B17="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="19" t="str">
+        <f aca="false">IF($B17="-", "-", ROUNDUP($I17/$F17,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I17" s="20" t="str">
+        <f aca="false">IF($B17="-", "-", $N17-$L17)</f>
+        <v>-</v>
+      </c>
+      <c r="J17" s="20"/>
+      <c r="K17" s="21" t="str">
+        <f aca="false">IF($B17="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L17" s="20" t="str">
+        <f aca="false">IF($B17="-", "-", ROUNDUP($N17/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M17" s="20"/>
+      <c r="N17" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O17" s="20"/>
+      <c r="P17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="15"/>
+      <c r="R17" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S17" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T17" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1519,42 +1553,47 @@
       </c>
       <c r="C18" s="9"/>
       <c r="D18" s="9"/>
-      <c r="E18" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G18" s="17"/>
-      <c r="H18" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I18" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J18" s="19"/>
-      <c r="K18" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L18" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M18" s="19"/>
-      <c r="N18" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O18" s="19"/>
-      <c r="P18" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q18" s="14"/>
-      <c r="R18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S18" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T18" s="14" t="s">
+      <c r="E18" s="17" t="str">
+        <f aca="false">IF($B18="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F18" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="19" t="str">
+        <f aca="false">IF($B18="-", "-", ROUNDUP($I18/$F18,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I18" s="20" t="str">
+        <f aca="false">IF($B18="-", "-", $N18-$L18)</f>
+        <v>-</v>
+      </c>
+      <c r="J18" s="20"/>
+      <c r="K18" s="21" t="str">
+        <f aca="false">IF($B18="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L18" s="20" t="str">
+        <f aca="false">IF($B18="-", "-", ROUNDUP($N18/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M18" s="20"/>
+      <c r="N18" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O18" s="20"/>
+      <c r="P18" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q18" s="15"/>
+      <c r="R18" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S18" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T18" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1564,42 +1603,47 @@
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
-      <c r="E19" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G19" s="17"/>
-      <c r="H19" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I19" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J19" s="19"/>
-      <c r="K19" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L19" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M19" s="19"/>
-      <c r="N19" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O19" s="19"/>
-      <c r="P19" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q19" s="14"/>
-      <c r="R19" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S19" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T19" s="14" t="s">
+      <c r="E19" s="17" t="str">
+        <f aca="false">IF($B19="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F19" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="19" t="str">
+        <f aca="false">IF($B19="-", "-", ROUNDUP($I19/$F19,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I19" s="20" t="str">
+        <f aca="false">IF($B19="-", "-", $N19-$L19)</f>
+        <v>-</v>
+      </c>
+      <c r="J19" s="20"/>
+      <c r="K19" s="21" t="str">
+        <f aca="false">IF($B19="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L19" s="20" t="str">
+        <f aca="false">IF($B19="-", "-", ROUNDUP($N19/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M19" s="20"/>
+      <c r="N19" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O19" s="20"/>
+      <c r="P19" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S19" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T19" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1609,42 +1653,47 @@
       </c>
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
-      <c r="E20" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F20" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G20" s="17"/>
-      <c r="H20" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J20" s="19"/>
-      <c r="K20" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L20" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M20" s="19"/>
-      <c r="N20" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O20" s="19"/>
-      <c r="P20" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q20" s="14"/>
-      <c r="R20" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S20" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T20" s="14" t="s">
+      <c r="E20" s="17" t="str">
+        <f aca="false">IF($B20="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="19" t="str">
+        <f aca="false">IF($B20="-", "-", ROUNDUP($I20/$F20,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I20" s="20" t="str">
+        <f aca="false">IF($B20="-", "-", $N20-$L20)</f>
+        <v>-</v>
+      </c>
+      <c r="J20" s="20"/>
+      <c r="K20" s="21" t="str">
+        <f aca="false">IF($B20="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L20" s="20" t="str">
+        <f aca="false">IF($B20="-", "-", ROUNDUP($N20/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M20" s="20"/>
+      <c r="N20" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O20" s="20"/>
+      <c r="P20" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S20" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T20" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1654,42 +1703,47 @@
       </c>
       <c r="C21" s="9"/>
       <c r="D21" s="9"/>
-      <c r="E21" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G21" s="17"/>
-      <c r="H21" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J21" s="19"/>
-      <c r="K21" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L21" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M21" s="19"/>
-      <c r="N21" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O21" s="19"/>
-      <c r="P21" s="14" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q21" s="14"/>
-      <c r="R21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S21" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T21" s="14" t="s">
+      <c r="E21" s="17" t="str">
+        <f aca="false">IF($B21="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="19" t="str">
+        <f aca="false">IF($B21="-", "-", ROUNDUP($I21/$F21,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I21" s="20" t="str">
+        <f aca="false">IF($B21="-", "-", $N21-$L21)</f>
+        <v>-</v>
+      </c>
+      <c r="J21" s="20"/>
+      <c r="K21" s="21" t="str">
+        <f aca="false">IF($B21="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L21" s="20" t="str">
+        <f aca="false">IF($B21="-", "-", ROUNDUP($N21/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M21" s="20"/>
+      <c r="N21" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O21" s="20"/>
+      <c r="P21" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q21" s="15"/>
+      <c r="R21" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S21" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T21" s="15" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1699,138 +1753,143 @@
       </c>
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
-      <c r="E22" s="16" t="s">
-        <v>2</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" s="17"/>
-      <c r="H22" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="I22" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="J22" s="19"/>
-      <c r="K22" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="L22" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="M22" s="19"/>
-      <c r="N22" s="19" t="s">
-        <v>2</v>
-      </c>
-      <c r="O22" s="19"/>
-      <c r="P22" s="14" t="s">
+      <c r="E22" s="17" t="str">
+        <f aca="false">IF($B22="-", "-", "buc.")</f>
+        <v>-</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="19" t="str">
+        <f aca="false">IF($B22="-", "-", ROUNDUP($I22/$F22,2))</f>
+        <v>-</v>
+      </c>
+      <c r="I22" s="20" t="str">
+        <f aca="false">IF($B22="-", "-", $N22-$L22)</f>
+        <v>-</v>
+      </c>
+      <c r="J22" s="20"/>
+      <c r="K22" s="21" t="str">
+        <f aca="false">IF($B22="-", "-", "20%")</f>
+        <v>-</v>
+      </c>
+      <c r="L22" s="20" t="str">
+        <f aca="false">IF($B22="-", "-", ROUNDUP($N22/6,2))</f>
+        <v>-</v>
+      </c>
+      <c r="M22" s="20"/>
+      <c r="N22" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="O22" s="20"/>
+      <c r="P22" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q22" s="15"/>
+      <c r="R22" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="S22" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="T22" s="15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B23" s="13"/>
+      <c r="C23" s="13"/>
+      <c r="D23" s="13"/>
+      <c r="E23" s="13"/>
+      <c r="F23" s="13"/>
+      <c r="G23" s="13"/>
+      <c r="H23" s="13"/>
+      <c r="I23" s="20" t="n">
+        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(I11:I22))</f>
+        <v>0</v>
+      </c>
+      <c r="J23" s="20"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="20" t="n">
+        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(L11:L22))</f>
+        <v>0</v>
+      </c>
+      <c r="M23" s="20"/>
+      <c r="N23" s="20" t="n">
+        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(N11:N22))</f>
+        <v>0</v>
+      </c>
+      <c r="O23" s="20"/>
+      <c r="P23" s="13"/>
+      <c r="Q23" s="13"/>
+      <c r="T23" s="22"/>
+    </row>
+    <row r="24" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B24" s="13"/>
+      <c r="C24" s="13"/>
+      <c r="D24" s="13"/>
+      <c r="E24" s="13"/>
+      <c r="F24" s="13"/>
+      <c r="G24" s="13"/>
+      <c r="H24" s="13"/>
+      <c r="I24" s="20" t="n">
+        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(I11:I22))</f>
+        <v>0</v>
+      </c>
+      <c r="J24" s="20"/>
+      <c r="K24" s="8"/>
+      <c r="L24" s="20" t="n">
+        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(L11:L22))</f>
+        <v>0</v>
+      </c>
+      <c r="M24" s="20"/>
+      <c r="N24" s="20" t="n">
+        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(N11:N22))</f>
+        <v>0</v>
+      </c>
+      <c r="O24" s="20"/>
+      <c r="T24" s="22"/>
+    </row>
+    <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C25" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="Q22" s="14"/>
-      <c r="R22" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="S22" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="T22" s="14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B23" s="12"/>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="12"/>
-      <c r="G23" s="12"/>
-      <c r="H23" s="12"/>
-      <c r="I23" s="19" t="n">
-        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(I11:I22))</f>
-        <v>50</v>
-      </c>
-      <c r="J23" s="19"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="19" t="n">
-        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(L11:L22))</f>
-        <v>10</v>
-      </c>
-      <c r="M23" s="19"/>
-      <c r="N23" s="19" t="n">
-        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(N11:N22))</f>
-        <v>60</v>
-      </c>
-      <c r="O23" s="19"/>
-      <c r="P23" s="12"/>
-      <c r="Q23" s="12"/>
-      <c r="T23" s="21"/>
-    </row>
-    <row r="24" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B24" s="12"/>
-      <c r="C24" s="12"/>
-      <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
-      <c r="G24" s="12"/>
-      <c r="H24" s="12"/>
-      <c r="I24" s="19" t="n">
-        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(I11:I22))</f>
-        <v>50</v>
-      </c>
-      <c r="J24" s="19"/>
-      <c r="K24" s="8"/>
-      <c r="L24" s="19" t="n">
-        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(L11:L22))</f>
-        <v>10</v>
-      </c>
-      <c r="M24" s="19"/>
-      <c r="N24" s="19" t="n">
-        <f aca="false">IF(COUNTBLANK( $B11:$B22)=12, "", SUM(N11:N22))</f>
-        <v>60</v>
-      </c>
-      <c r="O24" s="19"/>
-      <c r="T24" s="21"/>
-    </row>
-    <row r="25" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="K25" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L25" s="12"/>
+      <c r="M25" s="12"/>
+      <c r="N25" s="12"/>
+      <c r="O25" s="12"/>
+      <c r="P25" s="12"/>
+      <c r="Q25" s="12"/>
+      <c r="R25" s="12"/>
+      <c r="S25" s="12"/>
+      <c r="T25" s="12"/>
+    </row>
+    <row r="26" customFormat="false" ht="36.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="K26" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L26" s="12"/>
+      <c r="M26" s="12"/>
+      <c r="N26" s="12"/>
+      <c r="O26" s="12"/>
+      <c r="P26" s="12"/>
+      <c r="Q26" s="12"/>
+      <c r="R26" s="12"/>
+      <c r="S26" s="12"/>
+      <c r="T26" s="12"/>
+    </row>
+    <row r="27" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="C27" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="K25" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-    </row>
-    <row r="26" customFormat="false" ht="36.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K26" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-    </row>
-    <row r="27" customFormat="false" ht="14.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C27" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
       <c r="K27" s="8"/>
       <c r="L27" s="8"/>
       <c r="M27" s="8"/>
@@ -1843,18 +1902,18 @@
       <c r="T27" s="8"/>
     </row>
     <row r="28" customFormat="false" ht="25.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="K28" s="11" t="s">
-        <v>2</v>
-      </c>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
+      <c r="K28" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="L28" s="12"/>
+      <c r="M28" s="12"/>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12"/>
+      <c r="Q28" s="12"/>
+      <c r="R28" s="12"/>
+      <c r="S28" s="12"/>
+      <c r="T28" s="12"/>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="30" customFormat="false" ht="15.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
- Disabled deprecated Sensio "Router" annotation - Updated Invoice XLSX template: merged a couple of cells together; - Added maxlength validation to fiscalCode and vatNumber attributes of Company form - Disabled autocomplete for all text inputs in forms
</commit_message>
<xml_diff>
--- a/public/uploads/invoice/template.xlsx
+++ b/public/uploads/invoice/template.xlsx
@@ -274,6 +274,7 @@
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="7"/>
@@ -446,9 +447,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -458,7 +459,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -491,9 +492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -503,7 +504,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -536,9 +537,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -548,7 +549,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -581,9 +582,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -593,7 +594,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -626,9 +627,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -638,7 +639,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -671,9 +672,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -683,7 +684,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -716,9 +717,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -728,7 +729,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -761,9 +762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -773,7 +774,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -806,9 +807,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -818,7 +819,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -851,9 +852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -863,7 +864,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -896,9 +897,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -908,7 +909,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -941,9 +942,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>85320</xdr:colOff>
+      <xdr:colOff>84960</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180720</xdr:rowOff>
+      <xdr:rowOff>180360</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -953,7 +954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950400" cy="9673920"/>
+          <a:ext cx="9950040" cy="9673560"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -987,8 +988,8 @@
   </sheetPr>
   <dimension ref="B1:T43"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C28" activeCellId="0" sqref="C28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -997,7 +998,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="2.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8.71"/>
@@ -1011,6 +1012,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="4.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="3.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="18" style="0" width="5.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="21" style="0" width="8.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="90.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -1090,6 +1092,7 @@
       <c r="I5" s="9"/>
       <c r="J5" s="9"/>
       <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
       <c r="M5" s="8"/>
       <c r="N5" s="8"/>
       <c r="O5" s="10" t="s">
@@ -1113,6 +1116,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
       <c r="M6" s="8"/>
       <c r="N6" s="8"/>
       <c r="O6" s="10" t="s">
@@ -1935,9 +1939,9 @@
     <mergeCell ref="Q3:R3"/>
     <mergeCell ref="I4:L4"/>
     <mergeCell ref="O4:T4"/>
-    <mergeCell ref="C5:K5"/>
+    <mergeCell ref="C5:L5"/>
     <mergeCell ref="O5:T5"/>
-    <mergeCell ref="C6:K6"/>
+    <mergeCell ref="C6:L6"/>
     <mergeCell ref="O6:T6"/>
     <mergeCell ref="D7:D8"/>
     <mergeCell ref="F7:F8"/>

</xml_diff>

<commit_message>
- Updated XLS template - Updated InvoiceGenerator cells' data
</commit_message>
<xml_diff>
--- a/public/uploads/invoice/template.xlsx
+++ b/public/uploads/invoice/template.xlsx
@@ -447,9 +447,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -459,7 +459,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -492,9 +492,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -504,7 +504,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -537,9 +537,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -549,7 +549,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -582,9 +582,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -594,7 +594,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -627,9 +627,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -639,7 +639,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -672,9 +672,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -684,7 +684,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -717,9 +717,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -729,7 +729,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -762,9 +762,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -774,7 +774,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -807,9 +807,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -819,7 +819,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -852,9 +852,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -864,7 +864,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -897,9 +897,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -909,7 +909,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -942,9 +942,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>84960</xdr:colOff>
+      <xdr:colOff>84600</xdr:colOff>
       <xdr:row>41</xdr:row>
-      <xdr:rowOff>180360</xdr:rowOff>
+      <xdr:rowOff>180000</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -954,7 +954,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9950040" cy="9673560"/>
+          <a:ext cx="9950400" cy="9673200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -989,7 +989,7 @@
   <dimension ref="B1:T43"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="G9" activeCellId="0" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1947,7 +1947,7 @@
     <mergeCell ref="F7:F8"/>
     <mergeCell ref="M7:T8"/>
     <mergeCell ref="C9:D9"/>
-    <mergeCell ref="G9:J9"/>
+    <mergeCell ref="G9:K9"/>
     <mergeCell ref="N9:T9"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="F10:G10"/>

</xml_diff>